<commit_message>
aminokwasy: kodowanie i dekodowanie przechodzi testy bez sytuacji wyjatkowych
</commit_message>
<xml_diff>
--- a/Aminos.xlsx
+++ b/Aminos.xlsx
@@ -11,6 +11,9 @@
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Arkusz1!$AA$1:$AL$23</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -639,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y29"/>
+  <dimension ref="A1:AL50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,7 +653,7 @@
     <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -678,19 +681,19 @@
       <c r="J1" s="1"/>
       <c r="L1" s="1"/>
       <c r="N1" s="2" t="str">
-        <f>""""&amp;A1&amp;""""&amp;":"</f>
+        <f t="shared" ref="N1:N23" si="0">""""&amp;A1&amp;""""&amp;":"</f>
         <v>"GCU":</v>
       </c>
       <c r="O1" s="2" t="str">
-        <f>""""&amp;B1&amp;""""&amp;","</f>
+        <f t="shared" ref="O1:O23" si="1">""""&amp;B1&amp;""""&amp;","</f>
         <v>"A",</v>
       </c>
       <c r="P1" s="2" t="str">
-        <f>""""&amp;C1&amp;""""&amp;":"</f>
+        <f t="shared" ref="P1:P10" si="2">""""&amp;C1&amp;""""&amp;":"</f>
         <v>" GCC":</v>
       </c>
       <c r="Q1" s="2" t="str">
-        <f>""""&amp;D1&amp;""""&amp;","</f>
+        <f t="shared" ref="Q1:Q10" si="3">""""&amp;D1&amp;""""&amp;","</f>
         <v>"A",</v>
       </c>
       <c r="R1" s="2" t="str">
@@ -711,8 +714,18 @@
       </c>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -730,19 +743,19 @@
       <c r="J2" s="1"/>
       <c r="L2" s="1"/>
       <c r="N2" s="2" t="str">
-        <f>""""&amp;A2&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"UGU":</v>
       </c>
       <c r="O2" s="2" t="str">
-        <f>""""&amp;B2&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"C",</v>
       </c>
       <c r="P2" s="2" t="str">
-        <f>""""&amp;C2&amp;""""&amp;":"</f>
+        <f t="shared" si="2"/>
         <v>" UGC":</v>
       </c>
       <c r="Q2" s="2" t="str">
-        <f>""""&amp;D2&amp;""""&amp;","</f>
+        <f t="shared" si="3"/>
         <v>"C",</v>
       </c>
       <c r="R2" s="2"/>
@@ -751,8 +764,18 @@
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -770,19 +793,19 @@
       <c r="J3" s="1"/>
       <c r="L3" s="1"/>
       <c r="N3" s="2" t="str">
-        <f>""""&amp;A3&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"GAU":</v>
       </c>
       <c r="O3" s="2" t="str">
-        <f>""""&amp;B3&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"D",</v>
       </c>
       <c r="P3" s="2" t="str">
-        <f>""""&amp;C3&amp;""""&amp;":"</f>
+        <f t="shared" si="2"/>
         <v>" GAC":</v>
       </c>
       <c r="Q3" s="2" t="str">
-        <f>""""&amp;D3&amp;""""&amp;","</f>
+        <f t="shared" si="3"/>
         <v>"D",</v>
       </c>
       <c r="R3" s="2"/>
@@ -791,8 +814,18 @@
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -810,19 +843,19 @@
       <c r="J4" s="1"/>
       <c r="L4" s="1"/>
       <c r="N4" s="2" t="str">
-        <f>""""&amp;A4&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"GAA":</v>
       </c>
       <c r="O4" s="2" t="str">
-        <f>""""&amp;B4&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"E",</v>
       </c>
       <c r="P4" s="2" t="str">
-        <f>""""&amp;C4&amp;""""&amp;":"</f>
+        <f t="shared" si="2"/>
         <v>" GAG":</v>
       </c>
       <c r="Q4" s="2" t="str">
-        <f>""""&amp;D4&amp;""""&amp;","</f>
+        <f t="shared" si="3"/>
         <v>"E",</v>
       </c>
       <c r="R4" s="2"/>
@@ -831,8 +864,18 @@
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
@@ -850,19 +893,19 @@
       <c r="J5" s="1"/>
       <c r="L5" s="1"/>
       <c r="N5" s="2" t="str">
-        <f>""""&amp;A5&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"UUU":</v>
       </c>
       <c r="O5" s="2" t="str">
-        <f>""""&amp;B5&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"F",</v>
       </c>
       <c r="P5" s="2" t="str">
-        <f>""""&amp;C5&amp;""""&amp;":"</f>
+        <f t="shared" si="2"/>
         <v>" UUC":</v>
       </c>
       <c r="Q5" s="2" t="str">
-        <f>""""&amp;D5&amp;""""&amp;","</f>
+        <f t="shared" si="3"/>
         <v>"F",</v>
       </c>
       <c r="R5" s="2"/>
@@ -871,8 +914,18 @@
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
@@ -900,19 +953,19 @@
       <c r="J6" s="1"/>
       <c r="L6" s="1"/>
       <c r="N6" s="2" t="str">
-        <f>""""&amp;A6&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"GGU":</v>
       </c>
       <c r="O6" s="2" t="str">
-        <f>""""&amp;B6&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"G",</v>
       </c>
       <c r="P6" s="2" t="str">
-        <f>""""&amp;C6&amp;""""&amp;":"</f>
+        <f t="shared" si="2"/>
         <v>" GGC":</v>
       </c>
       <c r="Q6" s="2" t="str">
-        <f>""""&amp;D6&amp;""""&amp;","</f>
+        <f t="shared" si="3"/>
         <v>"G",</v>
       </c>
       <c r="R6" s="2" t="str">
@@ -933,8 +986,18 @@
       </c>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -952,19 +1015,19 @@
       <c r="J7" s="1"/>
       <c r="L7" s="1"/>
       <c r="N7" s="2" t="str">
-        <f>""""&amp;A7&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"CAU":</v>
       </c>
       <c r="O7" s="2" t="str">
-        <f>""""&amp;B7&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"H",</v>
       </c>
       <c r="P7" s="2" t="str">
-        <f>""""&amp;C7&amp;""""&amp;":"</f>
+        <f t="shared" si="2"/>
         <v>" CAC":</v>
       </c>
       <c r="Q7" s="2" t="str">
-        <f>""""&amp;D7&amp;""""&amp;","</f>
+        <f t="shared" si="3"/>
         <v>"H",</v>
       </c>
       <c r="R7" s="2"/>
@@ -973,8 +1036,18 @@
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -997,19 +1070,19 @@
       <c r="J8" s="1"/>
       <c r="L8" s="1"/>
       <c r="N8" s="2" t="str">
-        <f>""""&amp;A8&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"AUU":</v>
       </c>
       <c r="O8" s="2" t="str">
-        <f>""""&amp;B8&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"I",</v>
       </c>
       <c r="P8" s="2" t="str">
-        <f>""""&amp;C8&amp;""""&amp;":"</f>
+        <f t="shared" si="2"/>
         <v>" AUC":</v>
       </c>
       <c r="Q8" s="2" t="str">
-        <f>""""&amp;D8&amp;""""&amp;","</f>
+        <f t="shared" si="3"/>
         <v>"I",</v>
       </c>
       <c r="R8" s="2" t="str">
@@ -1024,8 +1097,18 @@
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -1043,19 +1126,19 @@
       <c r="J9" s="1"/>
       <c r="L9" s="1"/>
       <c r="N9" s="2" t="str">
-        <f>""""&amp;A9&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"AAA":</v>
       </c>
       <c r="O9" s="2" t="str">
-        <f>""""&amp;B9&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"K",</v>
       </c>
       <c r="P9" s="2" t="str">
-        <f>""""&amp;C9&amp;""""&amp;":"</f>
+        <f t="shared" si="2"/>
         <v>" AAG":</v>
       </c>
       <c r="Q9" s="2" t="str">
-        <f>""""&amp;D9&amp;""""&amp;","</f>
+        <f t="shared" si="3"/>
         <v>"K",</v>
       </c>
       <c r="R9" s="2"/>
@@ -1064,8 +1147,18 @@
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="2"/>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>48</v>
       </c>
@@ -1103,19 +1196,19 @@
         <v>9</v>
       </c>
       <c r="N10" s="2" t="str">
-        <f>""""&amp;A10&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"UUA":</v>
       </c>
       <c r="O10" s="2" t="str">
-        <f>""""&amp;B10&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"L",</v>
       </c>
       <c r="P10" s="2" t="str">
-        <f>""""&amp;C10&amp;""""&amp;":"</f>
+        <f t="shared" si="2"/>
         <v>" UUG":</v>
       </c>
       <c r="Q10" s="2" t="str">
-        <f>""""&amp;D10&amp;""""&amp;","</f>
+        <f t="shared" si="3"/>
         <v>"L",</v>
       </c>
       <c r="R10" s="2" t="str">
@@ -1150,8 +1243,20 @@
         <f>""""&amp;L10&amp;""""&amp;","</f>
         <v>"L",</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1164,11 +1269,11 @@
       <c r="J11" s="1"/>
       <c r="L11" s="1"/>
       <c r="N11" s="2" t="str">
-        <f>""""&amp;A11&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"AUG":</v>
       </c>
       <c r="O11" s="2" t="str">
-        <f>""""&amp;B11&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"M",</v>
       </c>
       <c r="P11" s="2"/>
@@ -1179,8 +1284,18 @@
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="2"/>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>54</v>
       </c>
@@ -1198,11 +1313,11 @@
       <c r="J12" s="1"/>
       <c r="L12" s="1"/>
       <c r="N12" s="2" t="str">
-        <f>""""&amp;A12&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"AAU":</v>
       </c>
       <c r="O12" s="2" t="str">
-        <f>""""&amp;B12&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"N",</v>
       </c>
       <c r="P12" s="2" t="str">
@@ -1219,8 +1334,18 @@
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="2"/>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -1233,11 +1358,11 @@
       <c r="J13" s="1"/>
       <c r="L13" s="1"/>
       <c r="N13" s="2" t="str">
-        <f>""""&amp;A13&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"UAG":</v>
       </c>
       <c r="O13" s="2" t="str">
-        <f>""""&amp;B13&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"O",</v>
       </c>
       <c r="P13" s="2"/>
@@ -1248,8 +1373,18 @@
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="2"/>
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="2"/>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>56</v>
       </c>
@@ -1277,11 +1412,11 @@
       <c r="J14" s="1"/>
       <c r="L14" s="1"/>
       <c r="N14" s="2" t="str">
-        <f>""""&amp;A14&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"CCU":</v>
       </c>
       <c r="O14" s="2" t="str">
-        <f>""""&amp;B14&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"P",</v>
       </c>
       <c r="P14" s="2" t="str">
@@ -1310,8 +1445,18 @@
       </c>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="2"/>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>60</v>
       </c>
@@ -1329,11 +1474,11 @@
       <c r="J15" s="1"/>
       <c r="L15" s="1"/>
       <c r="N15" s="2" t="str">
-        <f>""""&amp;A15&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"CAA":</v>
       </c>
       <c r="O15" s="2" t="str">
-        <f>""""&amp;B15&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"Q",</v>
       </c>
       <c r="P15" s="2" t="str">
@@ -1350,8 +1495,18 @@
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="2"/>
+      <c r="AH15" s="2"/>
+      <c r="AI15" s="2"/>
+      <c r="AJ15" s="2"/>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>62</v>
       </c>
@@ -1389,11 +1544,11 @@
         <v>16</v>
       </c>
       <c r="N16" s="2" t="str">
-        <f>""""&amp;A16&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"CGU":</v>
       </c>
       <c r="O16" s="2" t="str">
-        <f>""""&amp;B16&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"R",</v>
       </c>
       <c r="P16" s="2" t="str">
@@ -1436,8 +1591,20 @@
         <f>""""&amp;L16&amp;""""&amp;","</f>
         <v>"R",</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2"/>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2"/>
+      <c r="AJ16" s="2"/>
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="2"/>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>68</v>
       </c>
@@ -1475,11 +1642,11 @@
         <v>17</v>
       </c>
       <c r="N17" s="2" t="str">
-        <f>""""&amp;A17&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"UCU":</v>
       </c>
       <c r="O17" s="2" t="str">
-        <f>""""&amp;B17&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"S",</v>
       </c>
       <c r="P17" s="2" t="str">
@@ -1522,8 +1689,20 @@
         <f>""""&amp;L17&amp;""""&amp;","</f>
         <v>"S",</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="2"/>
+      <c r="AH17" s="2"/>
+      <c r="AI17" s="2"/>
+      <c r="AJ17" s="2"/>
+      <c r="AK17" s="2"/>
+      <c r="AL17" s="2"/>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>74</v>
       </c>
@@ -1551,11 +1730,11 @@
       <c r="J18" s="1"/>
       <c r="L18" s="1"/>
       <c r="N18" s="2" t="str">
-        <f>""""&amp;A18&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"ACU":</v>
       </c>
       <c r="O18" s="2" t="str">
-        <f>""""&amp;B18&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"T",</v>
       </c>
       <c r="P18" s="2" t="str">
@@ -1584,8 +1763,18 @@
       </c>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2"/>
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="2"/>
+      <c r="AJ18" s="2"/>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -1598,11 +1787,11 @@
       <c r="J19" s="1"/>
       <c r="L19" s="1"/>
       <c r="N19" s="2" t="str">
-        <f>""""&amp;A19&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"UGA":</v>
       </c>
       <c r="O19" s="2" t="str">
-        <f>""""&amp;B19&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"U",</v>
       </c>
       <c r="P19" s="2"/>
@@ -1613,8 +1802,18 @@
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2"/>
+      <c r="AH19" s="2"/>
+      <c r="AI19" s="2"/>
+      <c r="AJ19" s="2"/>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>78</v>
       </c>
@@ -1642,11 +1841,11 @@
       <c r="J20" s="1"/>
       <c r="L20" s="1"/>
       <c r="N20" s="2" t="str">
-        <f>""""&amp;A20&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"GUU":</v>
       </c>
       <c r="O20" s="2" t="str">
-        <f>""""&amp;B20&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"V",</v>
       </c>
       <c r="P20" s="2" t="str">
@@ -1675,8 +1874,18 @@
       </c>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="2"/>
+      <c r="AF20" s="2"/>
+      <c r="AG20" s="2"/>
+      <c r="AH20" s="2"/>
+      <c r="AI20" s="2"/>
+      <c r="AJ20" s="2"/>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1689,11 +1898,11 @@
       <c r="J21" s="1"/>
       <c r="L21" s="1"/>
       <c r="N21" s="2" t="str">
-        <f>""""&amp;A21&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"UGG":</v>
       </c>
       <c r="O21" s="2" t="str">
-        <f>""""&amp;B21&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"W",</v>
       </c>
       <c r="P21" s="2"/>
@@ -1704,8 +1913,18 @@
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="2"/>
+      <c r="AF21" s="2"/>
+      <c r="AG21" s="2"/>
+      <c r="AH21" s="2"/>
+      <c r="AI21" s="2"/>
+      <c r="AJ21" s="2"/>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>82</v>
       </c>
@@ -1723,11 +1942,11 @@
       <c r="J22" s="1"/>
       <c r="L22" s="1"/>
       <c r="N22" s="2" t="str">
-        <f>""""&amp;A22&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"UAU":</v>
       </c>
       <c r="O22" s="2" t="str">
-        <f>""""&amp;B22&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"Y",</v>
       </c>
       <c r="P22" s="2" t="str">
@@ -1744,8 +1963,18 @@
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2"/>
+      <c r="AH22" s="2"/>
+      <c r="AI22" s="2"/>
+      <c r="AJ22" s="2"/>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>84</v>
       </c>
@@ -1768,11 +1997,11 @@
       <c r="J23" s="1"/>
       <c r="L23" s="1"/>
       <c r="N23" s="2" t="str">
-        <f>""""&amp;A23&amp;""""&amp;":"</f>
+        <f t="shared" si="0"/>
         <v>"UAA":</v>
       </c>
       <c r="O23" s="2" t="str">
-        <f>""""&amp;B23&amp;""""&amp;","</f>
+        <f t="shared" si="1"/>
         <v>"-",</v>
       </c>
       <c r="P23" s="2" t="str">
@@ -1795,8 +2024,19 @@
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="2"/>
+      <c r="AI23" s="2"/>
+      <c r="AJ23" s="2"/>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="D28" s="1"/>
       <c r="P28" s="2" t="s">
         <v>89</v>
       </c>
@@ -1804,7 +2044,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="D29" s="1"/>
       <c r="P29">
         <f>COUNTA(N1:Y23)</f>
         <v>132</v>
@@ -1813,6 +2054,69 @@
         <f>66*2</f>
         <v>132</v>
       </c>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>